<commit_message>
First draft of paper WITHOUT Lit rev, results analysis
</commit_message>
<xml_diff>
--- a/Lit review and decisions/Selected Centralities.xlsx
+++ b/Lit review and decisions/Selected Centralities.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t xml:space="preserve">Degree Centrality </t>
   </si>
@@ -176,20 +175,6 @@
   </si>
   <si>
     <t>https://www.centiserver.org/centrality/Leverage_Centrality/</t>
-  </si>
-  <si>
-    <t>Information Centrality</t>
-  </si>
-  <si>
-    <t>Actor information centrality is a hybrid measure which relates to both path-length indices (e.g., closeness, graph centrality) and to walk-based eigenmeasures 
-(e.g., eigenvector centrality, Bonacich power). In particular, the information centrality of a given actor can be understood to be the harmonic average of the 
-“bandwidth” for all paths originating with said individual (where the bandwidth is taken to be inversely related to path length).</t>
-  </si>
-  <si>
-    <t>https://www.centiserver.org/centrality/Information_Centrality/</t>
-  </si>
-  <si>
-    <t>sna</t>
   </si>
   <si>
     <t>Local Bridging Centrality</t>
@@ -644,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,28 +648,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="185.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -889,44 +874,34 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>39</v>
-      </c>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -950,8 +925,7 @@
     <hyperlink ref="E9" r:id="rId7"/>
     <hyperlink ref="E10" r:id="rId8"/>
     <hyperlink ref="E11" r:id="rId9"/>
-    <hyperlink ref="E12" r:id="rId10"/>
-    <hyperlink ref="E13" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>